<commit_message>
added dump of db, new mcd and updated docs
</commit_message>
<xml_diff>
--- a/docs/planning.xlsx
+++ b/docs/planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\briangrn\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\briangrn\Documents\grin-eat-tpi2022\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD6651B-0DEB-4674-A1CA-2D4763A5985F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C6E4E5-989D-450F-9F95-7D277393B84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2655" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Immersion (Création git, vérifications du poste, temps pour adapt.)</t>
   </si>
   <si>
-    <t>Planification (se documenter, réflexions, croquis, remplir planning)</t>
-  </si>
-  <si>
     <t>DEVELOPPEMENT BACK END SERVEUR API (NODE JS)</t>
   </si>
   <si>
@@ -235,6 +232,12 @@
   </si>
   <si>
     <t>Mettre à jour l'affichage avec les nouvelles fonctionnalités implémentées</t>
+  </si>
+  <si>
+    <t>Planification &amp; Journal de bord (se documenter, réflexions, croquis, remplir planning)</t>
+  </si>
+  <si>
+    <t>Remplir la table countries avec un script qui récupère tout les pays de l'API restcountries</t>
   </si>
 </sst>
 </file>
@@ -590,11 +593,25 @@
   <dxfs count="83">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -623,6 +640,74 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -655,198 +740,116 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1510,14 +1513,18 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B28"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" customWidth="1"/>
-    <col min="3" max="27" width="10" customWidth="1"/>
+    <col min="1" max="1" width="68.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="27" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1649,7 +1656,7 @@
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="B4" s="34">
         <v>0.20833333333333334</v>
@@ -1713,7 +1720,7 @@
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="65"/>
       <c r="C6" s="66"/>
@@ -1734,7 +1741,7 @@
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="46">
         <v>6.25E-2</v>
@@ -1759,7 +1766,7 @@
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="46">
         <v>6.25E-2</v>
@@ -1786,7 +1793,7 @@
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="46">
         <v>6.25E-2</v>
@@ -1813,7 +1820,7 @@
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="46">
         <v>8.3333333333333329E-2</v>
@@ -1839,7 +1846,7 @@
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="46">
         <v>8.3333333333333329E-2</v>
@@ -1865,7 +1872,7 @@
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="46">
         <v>8.3333333333333329E-2</v>
@@ -1891,7 +1898,7 @@
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="46">
         <v>8.3333333333333329E-2</v>
@@ -1934,7 +1941,7 @@
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="65"/>
       <c r="C15" s="70"/>
@@ -1955,7 +1962,7 @@
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="46">
         <v>4.1666666666666664E-2</v>
@@ -1979,7 +1986,7 @@
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="46">
         <v>8.3333333333333329E-2</v>
@@ -2005,7 +2012,7 @@
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="46">
         <v>8.3333333333333329E-2</v>
@@ -2029,7 +2036,7 @@
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="46">
         <v>4.1666666666666664E-2</v>
@@ -2053,7 +2060,7 @@
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="46">
         <v>4.1666666666666664E-2</v>
@@ -2077,7 +2084,7 @@
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="46">
         <v>6.25E-2</v>
@@ -2101,7 +2108,7 @@
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="46">
         <v>0.16666666666666666</v>
@@ -2149,7 +2156,7 @@
     </row>
     <row r="24" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="64" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="65"/>
       <c r="C24" s="66"/>
@@ -2170,7 +2177,7 @@
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="46">
         <v>1.125</v>
@@ -2215,7 +2222,7 @@
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="46">
         <v>8.3333333333333329E-2</v>
@@ -2248,7 +2255,7 @@
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="59" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="46">
         <v>0.72916666666666663</v>
@@ -2291,7 +2298,7 @@
     </row>
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="53">
         <v>0.33333333333333331</v>
@@ -3515,14 +3522,17 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="27" width="10" customWidth="1"/>
+    <col min="3" max="3" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="27" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3617,7 +3627,7 @@
       <c r="C3" s="35">
         <v>3.125E-2</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="35"/>
       <c r="F3" s="43"/>
       <c r="G3" s="44"/>
@@ -3634,7 +3644,7 @@
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="B4" s="34">
         <v>0.20833333333333334</v>
@@ -3642,7 +3652,9 @@
       <c r="C4" s="35">
         <v>0.19791666666666666</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="36">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E4" s="35"/>
       <c r="F4" s="36"/>
       <c r="G4" s="35"/>
@@ -3654,7 +3666,7 @@
       <c r="M4" s="37"/>
       <c r="N4" s="10">
         <f>SUM(C4:M4)</f>
-        <v>0.19791666666666666</v>
+        <v>0.21875</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3672,13 +3684,13 @@
       <c r="L5" s="35"/>
       <c r="M5" s="37"/>
       <c r="N5" s="10">
-        <f t="shared" ref="N5:N13" si="0">SUM(C5:M5)</f>
+        <f>SUM(C5:M5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="65"/>
       <c r="C6" s="47"/>
@@ -3693,19 +3705,21 @@
       <c r="L6" s="47"/>
       <c r="M6" s="49"/>
       <c r="N6" s="10">
-        <f t="shared" si="0"/>
+        <f>SUM(C6:M6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="46">
         <v>6.25E-2</v>
       </c>
       <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
+      <c r="D7" s="48">
+        <v>5.5555555555555552E-2</v>
+      </c>
       <c r="E7" s="47"/>
       <c r="F7" s="48"/>
       <c r="G7" s="47"/>
@@ -3716,13 +3730,13 @@
       <c r="L7" s="47"/>
       <c r="M7" s="49"/>
       <c r="N7" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="N7:N13" si="0">SUM(C7:M7)</f>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="46">
         <v>6.25E-2</v>
@@ -3745,13 +3759,15 @@
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="46">
         <v>6.25E-2</v>
       </c>
       <c r="C9" s="47"/>
-      <c r="D9" s="48"/>
+      <c r="D9" s="48">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E9" s="47"/>
       <c r="F9" s="48"/>
       <c r="G9" s="47"/>
@@ -3763,12 +3779,12 @@
       <c r="M9" s="49"/>
       <c r="N9" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="46">
         <v>8.3333333333333329E-2</v>
@@ -3791,7 +3807,7 @@
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="46">
         <v>8.3333333333333329E-2</v>
@@ -3814,7 +3830,7 @@
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="46">
         <v>8.3333333333333329E-2</v>
@@ -3837,7 +3853,7 @@
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="46">
         <v>8.3333333333333329E-2</v>
@@ -3859,10 +3875,16 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60"/>
-      <c r="B14" s="34"/>
+      <c r="A14" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="34">
+        <v>1.7361111111111112E-2</v>
+      </c>
       <c r="C14" s="43"/>
-      <c r="D14" s="36"/>
+      <c r="D14" s="36">
+        <v>1.7361111111111112E-2</v>
+      </c>
       <c r="E14" s="43"/>
       <c r="F14" s="36"/>
       <c r="G14" s="43"/>
@@ -3874,12 +3896,12 @@
       <c r="M14" s="37"/>
       <c r="N14" s="10">
         <f>SUM(C14:M14)</f>
-        <v>0</v>
+        <v>1.7361111111111112E-2</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="65"/>
       <c r="C15" s="50"/>
@@ -3900,7 +3922,7 @@
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="46">
         <v>4.1666666666666664E-2</v>
@@ -3923,7 +3945,7 @@
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="46">
         <v>8.3333333333333329E-2</v>
@@ -3946,7 +3968,7 @@
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="46">
         <v>8.3333333333333329E-2</v>
@@ -3969,7 +3991,7 @@
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="46">
         <v>4.1666666666666664E-2</v>
@@ -3992,7 +4014,7 @@
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="46">
         <v>4.1666666666666664E-2</v>
@@ -4015,7 +4037,7 @@
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="46">
         <v>6.25E-2</v>
@@ -4038,7 +4060,7 @@
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="46">
         <v>0.16666666666666666</v>
@@ -4080,7 +4102,7 @@
     </row>
     <row r="24" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="64" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="65"/>
       <c r="C24" s="47"/>
@@ -4101,7 +4123,7 @@
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="46">
         <v>1.125</v>
@@ -4109,7 +4131,9 @@
       <c r="C25" s="47">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D25" s="48"/>
+      <c r="D25" s="48">
+        <v>0.19791666666666666</v>
+      </c>
       <c r="E25" s="50"/>
       <c r="F25" s="48"/>
       <c r="G25" s="50"/>
@@ -4121,12 +4145,12 @@
       <c r="M25" s="49"/>
       <c r="N25" s="10">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="46">
         <v>8.3333333333333329E-2</v>
@@ -4149,7 +4173,7 @@
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="59" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="46">
         <v>0.72916666666666663</v>
@@ -4172,7 +4196,7 @@
     </row>
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="53">
         <v>0.33333333333333331</v>
@@ -4196,7 +4220,7 @@
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10">
         <f t="shared" ref="B29:M29" si="2">SUM(B2:B28)</f>
-        <v>3.666666666666667</v>
+        <v>3.6840277777777781</v>
       </c>
       <c r="C29" s="10">
         <f t="shared" si="2"/>
@@ -4204,7 +4228,7 @@
       </c>
       <c r="D29" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E29" s="10">
         <f t="shared" si="2"/>
@@ -4246,11 +4270,11 @@
     <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M30" s="10">
         <f>SUM(C29:M29)</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="N30" s="10">
         <f>SUM(N2:N28)</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5311,43 +5335,43 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
+  <conditionalFormatting sqref="N2 N5">
     <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3">
+  <conditionalFormatting sqref="N3 N6">
     <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5:N13">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
-      <formula>$B5</formula>
+  <conditionalFormatting sqref="N7:N13">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+      <formula>$B7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:N28">
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
       <formula>$B15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:M29">
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>$B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>$B14</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7181,152 +7205,152 @@
     <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C2:J3 F27 H27:I27 C4:C22 E4:E22 G4:G22 I4:I22 L4:L22 C24:C25 G24:G25 I24:I25 I28:I29 E24:E25 L24:L25 L2:M3 L27:L29 E27:E29 G27:G29 C27:C29">
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="22" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:J3 C6:J13 C15:J22 C24:J25 L24:M25 L15:M22 L6:M13 L2:M3 L27:M29 C27:J29">
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="23" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23 I23 G23 E23 C23">
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="24" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:J23 L23:M23">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28 F28 H28 J28 M28">
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27 G27 J27">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:J25 L2:M25 L27:M29 C27:J29">
-    <cfRule type="cellIs" dxfId="24" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:J25 L2:M25 L27:M29 C27:J29">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:J25 L2:M25 L27:M29 C27:J29">
-    <cfRule type="cellIs" dxfId="22" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3">
-    <cfRule type="cellIs" dxfId="21" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3 K6:K13 K15:K22 K24:K25 K27:K29">
-    <cfRule type="cellIs" dxfId="20" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="19" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K25 K27:K29">
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K25 K27:K29">
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="20" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K25 K27:K29">
-    <cfRule type="cellIs" dxfId="14" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:N13">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>$B5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:N25 N27:N29">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>$B15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:M30">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26 E26 G26 I26 L26">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:J26 L26:M26">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:J26 L26:M26">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:J26 L26:M26">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update docs day 4
</commit_message>
<xml_diff>
--- a/docs/planning.xlsx
+++ b/docs/planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\briangrn\Documents\grin-eat-tpi2022\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF121CA-18F6-4A7C-A321-053428A1E02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836D40DE-6A52-4E1A-A96C-347B661646DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2655" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,8 +199,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +232,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -484,6 +495,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1160,7 +1172,7 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3169,7 +3181,7 @@
   <dimension ref="A1:AA1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3310,7 +3322,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="F4" s="9">
-        <v>1.0416666666666666E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
@@ -3321,7 +3333,7 @@
       <c r="M4" s="10"/>
       <c r="N4" s="6">
         <f>SUM(C4:M4)</f>
-        <v>0.25</v>
+        <v>0.25347222222222221</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3573,7 +3585,7 @@
       <c r="D15" s="9"/>
       <c r="E15" s="16"/>
       <c r="F15" s="9">
-        <v>2.0833333333333332E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="9"/>
@@ -3584,7 +3596,7 @@
       <c r="M15" s="10"/>
       <c r="N15" s="6">
         <f>SUM(C15:M15)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3596,7 +3608,7 @@
       <c r="D16" s="9"/>
       <c r="E16" s="16"/>
       <c r="F16" s="9">
-        <v>0.11458333333333333</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="9"/>
@@ -3849,7 +3861,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="46" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="19">
@@ -3864,7 +3876,9 @@
       <c r="E28" s="20">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F28" s="21"/>
+      <c r="F28" s="21">
+        <v>3.125E-2</v>
+      </c>
       <c r="G28" s="23"/>
       <c r="H28" s="21"/>
       <c r="I28" s="20"/>
@@ -3874,7 +3888,7 @@
       <c r="M28" s="22"/>
       <c r="N28" s="6">
         <f t="shared" si="1"/>
-        <v>0.32291666666666669</v>
+        <v>0.35416666666666669</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3913,7 +3927,7 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="F30" s="20">
-        <v>1.0416666666666666E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
@@ -3924,7 +3938,7 @@
       <c r="M30" s="25"/>
       <c r="N30" s="6">
         <f t="shared" si="1"/>
-        <v>0.11458333333333334</v>
+        <v>0.16666666666666669</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3969,7 +3983,7 @@
       </c>
       <c r="F32" s="6">
         <f t="shared" si="2"/>
-        <v>0.20486111111111108</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="G32" s="6">
         <f t="shared" si="2"/>
@@ -4003,11 +4017,11 @@
     <row r="33" spans="13:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M33" s="6">
         <f>SUM(C32:M32)</f>
-        <v>1.2048611111111112</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="N33" s="6">
         <f>SUM(N2:N31)</f>
-        <v>1.0902777777777779</v>
+        <v>1.1875000000000002</v>
       </c>
     </row>
     <row r="34" spans="13:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
new css removed bootstrap menu page done update of docs
</commit_message>
<xml_diff>
--- a/docs/planning.xlsx
+++ b/docs/planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\briangrn\Documents\grin-eat-tpi2022\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\html\grin-eat-tpi2022\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1A1158-93D1-4341-B595-E62C6E9F39E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA55CDC-D0D0-4BBD-BC81-FCB7EE3CBDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2655" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="2910" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Page des menus des restaurants</t>
+  </si>
+  <si>
+    <t>Modifier le serveur pour accepté soit une adresse soit des coordonnées (latitude/longitude)</t>
+  </si>
+  <si>
+    <t>Recherche avec ou sans autocomplete (coordonnées ou adresse si sans autocomplete)</t>
   </si>
 </sst>
 </file>
@@ -435,7 +441,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -498,6 +504,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3183,12 +3190,12 @@
   <dimension ref="A1:AA1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.875" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="6.25" bestFit="1" customWidth="1"/>
@@ -3306,13 +3313,15 @@
       <c r="I3" s="8">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="J3" s="16"/>
+      <c r="J3" s="8">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
       <c r="M3" s="17"/>
       <c r="N3" s="6">
         <f>SUM(C3:M3)</f>
-        <v>6.2500000000000014E-2</v>
+        <v>6.9444444444444461E-2</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3343,13 +3352,19 @@
       <c r="I4" s="8">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="8"/>
+      <c r="J4" s="9">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="K4" s="9">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="L4" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="M4" s="10"/>
       <c r="N4" s="6">
         <f>SUM(C4:M4)</f>
-        <v>0.29166666666666669</v>
+        <v>0.31944444444444448</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3642,7 +3657,9 @@
       <c r="N16" s="6"/>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="46" t="s">
+        <v>42</v>
+      </c>
       <c r="B17" s="7"/>
       <c r="C17" s="16"/>
       <c r="D17" s="9"/>
@@ -3652,12 +3669,14 @@
       <c r="H17" s="9"/>
       <c r="I17" s="16"/>
       <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
+      <c r="K17" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="L17" s="16"/>
       <c r="M17" s="10"/>
       <c r="N17" s="6">
         <f>SUM(C17:M17)</f>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3844,7 +3863,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="43" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="18">
@@ -3859,15 +3878,19 @@
       <c r="I25" s="19"/>
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
-      <c r="L25" s="19"/>
+      <c r="L25" s="19">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="M25" s="21"/>
       <c r="N25" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+      <c r="A26" s="43" t="s">
+        <v>43</v>
+      </c>
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
       <c r="D26" s="20"/>
@@ -3877,12 +3900,14 @@
       <c r="H26" s="20"/>
       <c r="I26" s="19"/>
       <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="K26" s="20">
+        <v>3.125E-2</v>
+      </c>
       <c r="L26" s="19"/>
       <c r="M26" s="21"/>
       <c r="N26" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3934,13 +3959,19 @@
       <c r="I28" s="19">
         <v>0.13541666666666666</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="19"/>
+      <c r="J28" s="20">
+        <v>0.125</v>
+      </c>
+      <c r="K28" s="20">
+        <v>0.125</v>
+      </c>
+      <c r="L28" s="19">
+        <v>0.17708333333333334</v>
+      </c>
       <c r="M28" s="21"/>
       <c r="N28" s="6">
         <f t="shared" si="1"/>
-        <v>0.63541666666666663</v>
+        <v>1.0625</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3986,13 +4017,15 @@
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
+      <c r="J30" s="19">
+        <v>9.0277777777777776E-2</v>
+      </c>
       <c r="K30" s="19"/>
       <c r="L30" s="19"/>
       <c r="M30" s="24"/>
       <c r="N30" s="6">
         <f t="shared" si="1"/>
-        <v>0.14583333333333334</v>
+        <v>0.2361111111111111</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4017,13 +4050,19 @@
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="I31" s="26"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="28"/>
+      <c r="J31" s="27">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="K31" s="27">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="L31" s="28">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="M31" s="29"/>
       <c r="N31" s="6">
         <f t="shared" si="1"/>
-        <v>9.0277777777777776E-2</v>
+        <v>0.31944444444444448</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4061,15 +4100,15 @@
       </c>
       <c r="J32" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="K32" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="M32" s="6">
         <f t="shared" si="2"/>
@@ -4079,11 +4118,11 @@
     <row r="33" spans="13:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M33" s="6">
         <f>SUM(C32:M32)</f>
-        <v>2.3333333333333335</v>
+        <v>3.3333333333333339</v>
       </c>
       <c r="N33" s="6">
         <f>SUM(N2:N31)</f>
-        <v>2.1875000000000004</v>
+        <v>3.1875000000000004</v>
       </c>
     </row>
     <row r="34" spans="13:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
last dump, update docs, dev part done
</commit_message>
<xml_diff>
--- a/docs/planning.xlsx
+++ b/docs/planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\html\grin-eat-tpi2022\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\briangrn\Documents\grin-eat-tpi2022\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA55CDC-D0D0-4BBD-BC81-FCB7EE3CBDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2D359F-D4F6-4F27-970E-B070F5FC00D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="2910" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="2910" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -35,45 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Tâches à réaliser</t>
   </si>
   <si>
     <t>Temps nécessaire</t>
-  </si>
-  <si>
-    <t>1er jour</t>
-  </si>
-  <si>
-    <t>2e jour</t>
-  </si>
-  <si>
-    <t>3e jour</t>
-  </si>
-  <si>
-    <t>4e jour</t>
-  </si>
-  <si>
-    <t>5e jour</t>
-  </si>
-  <si>
-    <t>6e jour</t>
-  </si>
-  <si>
-    <t>7e jour</t>
-  </si>
-  <si>
-    <t>8e jour</t>
-  </si>
-  <si>
-    <t>9e jour</t>
-  </si>
-  <si>
-    <t>10e jour</t>
-  </si>
-  <si>
-    <t>11e jour</t>
   </si>
   <si>
     <t>Total</t>
@@ -214,7 +181,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,18 +207,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -286,17 +247,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -436,12 +386,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -449,62 +427,61 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1178,19 +1155,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="68.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.25" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="8.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.875" bestFit="1" customWidth="1"/>
     <col min="15" max="27" width="10" customWidth="1"/>
   </cols>
@@ -1202,867 +1180,867 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="47">
+        <v>44683</v>
+      </c>
+      <c r="D1" s="47">
+        <v>44684</v>
+      </c>
+      <c r="E1" s="47">
+        <v>44685</v>
+      </c>
+      <c r="F1" s="47">
+        <v>44686</v>
+      </c>
+      <c r="G1" s="47">
+        <v>44690</v>
+      </c>
+      <c r="H1" s="47">
+        <v>44691</v>
+      </c>
+      <c r="I1" s="47">
+        <v>44692</v>
+      </c>
+      <c r="J1" s="47">
+        <v>44693</v>
+      </c>
+      <c r="K1" s="47">
+        <v>44697</v>
+      </c>
+      <c r="L1" s="47">
+        <v>44698</v>
+      </c>
+      <c r="M1" s="47">
+        <v>44699</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+    </row>
+    <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-    </row>
-    <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>6.25E-2</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="10">
         <v>6.25E-2</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="6">
+      <c r="D2" s="11"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="4">
         <f>SUM(C2:M2)</f>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7">
+      <c r="A3" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="6">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <v>6.9444444444444397E-3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="6">
         <v>6.9444444444444397E-3</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="6">
         <v>6.9444444444444397E-3</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="6">
         <v>6.9444444444444397E-3</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="6">
         <v>6.9444444444444397E-3</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="6">
         <v>6.9444444444444397E-3</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="6">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="6">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="N3" s="41">
+      <c r="N3" s="39">
         <f>SUM(C3:M3)</f>
         <v>8.3333333333333301E-2</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="7">
+      <c r="A4" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="7">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="6">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="7">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="6">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="8">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="4">
         <f>SUM(C4:M4)</f>
         <v>0.20833333333333337</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="6">
+      <c r="A5" s="31"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="4">
         <f t="shared" ref="N5:N13" si="0">SUM(C5:M5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="6">
+      <c r="A6" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="18">
+      <c r="A7" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16">
         <v>6.25E-2</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20">
+      <c r="C7" s="17"/>
+      <c r="D7" s="18">
         <v>6.25E-2</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="6">
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="4">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="18">
+      <c r="A8" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16">
         <v>6.25E-2</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20">
+      <c r="C8" s="17"/>
+      <c r="D8" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="6">
+      <c r="F8" s="18"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="4">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="18">
+      <c r="A9" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16">
         <v>6.25E-2</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20">
+      <c r="C9" s="17"/>
+      <c r="D9" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="6">
+      <c r="F9" s="18"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="4">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="18">
+      <c r="A10" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="20"/>
-      <c r="F10" s="19">
+      <c r="C10" s="20"/>
+      <c r="D10" s="18"/>
+      <c r="F10" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="6">
+      <c r="H10" s="20"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="4">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="18">
+      <c r="A11" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="20"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20">
+      <c r="C11" s="20"/>
+      <c r="D11" s="18"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="6">
+      <c r="I11" s="18"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="4">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="18">
+      <c r="A12" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="20"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="20">
+      <c r="C12" s="20"/>
+      <c r="D12" s="18"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="K12" s="20"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="6">
+      <c r="K12" s="18"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="4">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="18">
+      <c r="A13" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="20"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="20">
+      <c r="C13" s="20"/>
+      <c r="D13" s="18"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="18">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="L13" s="22"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="6">
+      <c r="L13" s="20"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="4">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="6">
+      <c r="A14" s="30"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="4">
         <f>SUM(C14:M14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="6">
+      <c r="A15" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="4">
         <f t="shared" ref="N15:N28" si="1">SUM(C15:M15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="18">
+      <c r="A16" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="16">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="20"/>
-      <c r="F16" s="19">
+      <c r="C16" s="20"/>
+      <c r="D16" s="18"/>
+      <c r="F16" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="6">
+      <c r="G16" s="18"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="4">
         <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="18">
+      <c r="A17" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="20"/>
-      <c r="F17" s="19">
+      <c r="C17" s="20"/>
+      <c r="D17" s="18"/>
+      <c r="F17" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="6">
+      <c r="H17" s="17"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="4">
         <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="18">
+      <c r="A18" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="19">
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="6">
+      <c r="I18" s="18"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="4">
         <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="18">
+      <c r="A19" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="16">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="20">
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="6">
+      <c r="J19" s="17"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="4">
         <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="18">
+      <c r="A20" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="16">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="20">
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="6">
+      <c r="J20" s="17"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="4">
         <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="18">
+      <c r="A21" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="16">
         <v>6.25E-2</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="19">
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="17">
         <v>6.25E-2</v>
       </c>
-      <c r="K21" s="20"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="6">
+      <c r="K21" s="18"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="4">
         <f t="shared" si="1"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="18">
+      <c r="A22" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="16">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20">
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G22" s="19"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20">
+      <c r="G22" s="17"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18">
         <v>4.8611111111111112E-2</v>
       </c>
-      <c r="L22" s="19">
+      <c r="L22" s="17">
         <v>9.7222222222222224E-2</v>
       </c>
-      <c r="M22" s="21"/>
-      <c r="N22" s="6">
+      <c r="M22" s="19"/>
+      <c r="N22" s="4">
         <f t="shared" si="1"/>
         <v>0.16666666666666669</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="6">
+      <c r="A23" s="29"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="6">
+      <c r="A24" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="35"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="18">
+      <c r="A25" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="16">
         <v>1.125</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="17">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="17">
         <v>0.125</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="17">
         <v>0.125</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="H25" s="19">
+      <c r="H25" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="I25" s="19">
+      <c r="I25" s="17">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="J25" s="19">
+      <c r="J25" s="17">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="K25" s="19">
+      <c r="K25" s="17">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="L25" s="19">
+      <c r="L25" s="17">
         <v>0.125</v>
       </c>
-      <c r="M25" s="19">
+      <c r="M25" s="17">
         <v>0.125</v>
       </c>
-      <c r="N25" s="6">
+      <c r="N25" s="4">
         <f>SUM(C25:M25)</f>
         <v>1.1249999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="18">
+      <c r="A26" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19">
+      <c r="C26" s="17"/>
+      <c r="D26" s="17">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19">
+      <c r="E26" s="17"/>
+      <c r="F26" s="17">
         <f>TIME(0,30,0)</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19">
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17">
         <f>TIME(0,30,0)</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19">
+      <c r="K26" s="17"/>
+      <c r="L26" s="17">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="M26" s="21"/>
-      <c r="N26" s="6">
+      <c r="M26" s="19"/>
+      <c r="N26" s="4">
         <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="18">
+      <c r="A27" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="16">
         <v>0.72916666666666663</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F27" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="H27" s="19">
+      <c r="H27" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="I27" s="19">
+      <c r="I27" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="K27" s="19">
+      <c r="K27" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="L27" s="19">
+      <c r="L27" s="17">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="M27" s="24">
+      <c r="M27" s="22">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="N27" s="6">
+      <c r="N27" s="4">
         <f t="shared" si="1"/>
         <v>0.72916666666666674</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="25">
+      <c r="A28" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="23">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="27">
+      <c r="C28" s="24"/>
+      <c r="D28" s="25">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E28" s="28">
+      <c r="E28" s="26">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="25">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G28" s="28">
+      <c r="G28" s="26">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28" s="25">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="I28" s="28">
+      <c r="I28" s="26">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="J28" s="27">
+      <c r="J28" s="25">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="K28" s="27">
+      <c r="K28" s="25">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="L28" s="28">
+      <c r="L28" s="26">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="M28" s="29">
+      <c r="M28" s="27">
         <v>0.14583333333333334</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N28" s="4">
         <f t="shared" si="1"/>
         <v>0.33333333333333337</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="6">
+      <c r="B29" s="4">
         <f t="shared" ref="B29:M29" si="2">SUM(B2:B28)</f>
         <v>3.666666666666667</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="J29" s="6">
+      <c r="J29" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K29" s="6">
+      <c r="K29" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="L29" s="6">
+      <c r="L29" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="M29" s="6">
+      <c r="M29" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333337</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M30" s="6">
+      <c r="M30" s="4">
         <f>SUM(C29:M29)</f>
         <v>3.666666666666667</v>
       </c>
-      <c r="N30" s="6">
+      <c r="N30" s="4">
         <f>SUM(N2:N28)</f>
         <v>3.6666666666666674</v>
       </c>
@@ -3180,8 +3158,8 @@
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="68" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3189,19 +3167,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="73.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="8.875" bestFit="1" customWidth="1"/>
     <col min="14" max="27" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3212,917 +3186,932 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="47">
+        <v>44683</v>
+      </c>
+      <c r="D1" s="47">
+        <v>44684</v>
+      </c>
+      <c r="E1" s="47">
+        <v>44685</v>
+      </c>
+      <c r="F1" s="47">
+        <v>44686</v>
+      </c>
+      <c r="G1" s="47">
+        <v>44690</v>
+      </c>
+      <c r="H1" s="47">
+        <v>44691</v>
+      </c>
+      <c r="I1" s="47">
+        <v>44692</v>
+      </c>
+      <c r="J1" s="47">
+        <v>44693</v>
+      </c>
+      <c r="K1" s="47">
+        <v>44697</v>
+      </c>
+      <c r="L1" s="47">
+        <v>44698</v>
+      </c>
+      <c r="M1" s="47">
+        <v>44699</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+    </row>
+    <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-    </row>
-    <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>6.25E-2</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="10">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="6">
+      <c r="D2" s="11"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="4">
         <f>SUM(C2:M2)</f>
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7">
+      <c r="A3" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>3.125E-2</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="6">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="6">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="6">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="6">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="6">
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="4">
         <f>SUM(C3:M3)</f>
         <v>6.9444444444444461E-2</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="7">
+      <c r="A4" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>0.19791666666666666</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="7">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="6">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="6">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="6">
+      <c r="M4" s="8"/>
+      <c r="N4" s="4">
         <f>SUM(C4:M4)</f>
         <v>0.31944444444444448</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="6">
+      <c r="A5" s="31"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="4">
         <f>SUM(C5:M5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="6">
+      <c r="A6" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="4">
         <f>SUM(C6:M6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="18">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16">
         <v>6.25E-2</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20">
+      <c r="C7" s="17"/>
+      <c r="D7" s="18">
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="20">
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="17">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="6">
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="4">
         <f t="shared" ref="N7:N13" si="0">SUM(C7:M7)</f>
         <v>9.0277777777777776E-2</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="18">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16">
         <v>6.25E-2</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="19">
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="17">
         <v>6.25E-2</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="6">
+      <c r="F8" s="18"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="4">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="18">
+      <c r="A9" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16">
         <v>6.25E-2</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20">
+      <c r="C9" s="17"/>
+      <c r="D9" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="6">
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="4">
         <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="18">
+      <c r="A10" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="19">
+      <c r="C10" s="20"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="17">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="6">
+      <c r="F10" s="18"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="4">
         <f t="shared" si="0"/>
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="18">
+      <c r="A11" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="19">
+      <c r="C11" s="20"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="17">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="6">
+      <c r="F11" s="18"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="4">
         <f t="shared" si="0"/>
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="18">
+      <c r="A12" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="19">
+      <c r="C12" s="20"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="17">
         <v>6.25E-2</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="6">
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="4">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="18">
+      <c r="A13" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="19">
+      <c r="C13" s="20"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="17">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="6">
+      <c r="G13" s="20"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="4">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="7">
+      <c r="A14" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="5">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="9">
+      <c r="C14" s="14"/>
+      <c r="D14" s="7">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="6">
+      <c r="E14" s="14"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="4">
         <f>SUM(C14:M14)</f>
         <v>1.7361111111111112E-2</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="9">
+      <c r="A15" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="5">
         <v>3.125E-2</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="6">
+      <c r="C15" s="14"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="7">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="4">
         <f>SUM(C15:M15)</f>
         <v>3.125E-2</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="9">
+      <c r="A16" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="5">
         <v>0.14583333333333334</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="6"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="7">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="4">
+        <f>SUM(C16:M16)</f>
+        <v>0.14583333333333334</v>
+      </c>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9">
+      <c r="A17" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="6">
+      <c r="C17" s="14"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="L17" s="14"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="4">
         <f>SUM(C17:M17)</f>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="6">
+      <c r="A18" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="35"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="4">
         <f t="shared" ref="N18:N31" si="1">SUM(C18:M18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="18">
+        <v>19</v>
+      </c>
+      <c r="B19" s="16">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="19">
+      <c r="C19" s="20"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="17">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="6">
+      <c r="H19" s="18"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="4">
         <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="18">
+      <c r="A20" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="19">
+      <c r="C20" s="20"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="H20" s="20">
+      <c r="H20" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="17">
         <v>3.125E-2</v>
       </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="6">
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="4">
         <f t="shared" si="1"/>
         <v>9.375E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="18">
+      <c r="A21" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="19">
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="18">
         <v>6.25E-2</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="6">
+      <c r="I21" s="17"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="4">
         <f t="shared" si="1"/>
         <v>0.10416666666666666</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="18">
+      <c r="A22" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="16">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="20">
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="17">
         <v>3.125E-2</v>
       </c>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="6">
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="4">
         <f t="shared" si="1"/>
         <v>5.2083333333333329E-2</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="18">
+      <c r="A23" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="16">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="20">
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="17">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="6">
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="4">
         <f t="shared" si="1"/>
         <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="18">
+      <c r="A24" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="16">
         <v>6.25E-2</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="20">
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="17">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="6">
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="4">
         <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="18">
+      <c r="A25" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="19">
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="17">
         <v>0.10416666666666667</v>
       </c>
-      <c r="M25" s="21"/>
-      <c r="N25" s="6">
+      <c r="M25" s="19"/>
+      <c r="N25" s="4">
         <f t="shared" si="1"/>
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20">
+      <c r="A26" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18">
         <v>3.125E-2</v>
       </c>
-      <c r="L26" s="19"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="6">
+      <c r="L26" s="17"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="4">
         <f t="shared" si="1"/>
         <v>3.125E-2</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="6">
+      <c r="A27" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="35"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="18">
+      <c r="A28" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="16">
         <v>1.125</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="18">
         <v>0.19791666666666666</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F28" s="18">
         <v>3.125E-2</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="17">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H28" s="20">
+      <c r="H28" s="18">
         <v>0.125</v>
       </c>
-      <c r="I28" s="19">
+      <c r="I28" s="17">
         <v>0.13541666666666666</v>
       </c>
-      <c r="J28" s="20">
+      <c r="J28" s="18">
         <v>0.125</v>
       </c>
-      <c r="K28" s="20">
+      <c r="K28" s="18">
         <v>0.125</v>
       </c>
-      <c r="L28" s="19">
-        <v>0.17708333333333334</v>
-      </c>
-      <c r="M28" s="21"/>
-      <c r="N28" s="6">
+      <c r="L28" s="17">
+        <v>9.375E-2</v>
+      </c>
+      <c r="M28" s="19">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="N28" s="4">
         <f t="shared" si="1"/>
-        <v>1.0625</v>
+        <v>1.1875</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="18">
+      <c r="A29" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="6">
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="19">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="N29" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="18">
+      <c r="A30" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="16">
         <v>0.72916666666666663</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19">
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="17">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19">
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17">
         <v>9.0277777777777776E-2</v>
       </c>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="6">
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="4">
         <f t="shared" si="1"/>
         <v>0.2361111111111111</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="25">
+      <c r="A31" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="23">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="28">
+      <c r="C31" s="24"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="26">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="25">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G31" s="28">
+      <c r="G31" s="26">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H31" s="27">
+      <c r="H31" s="25">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="I31" s="26"/>
-      <c r="J31" s="27">
+      <c r="I31" s="24"/>
+      <c r="J31" s="25">
         <v>0.10416666666666667</v>
       </c>
-      <c r="K31" s="27">
+      <c r="K31" s="25">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="L31" s="28">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M31" s="29"/>
-      <c r="N31" s="6">
+      <c r="L31" s="26">
+        <v>0.125</v>
+      </c>
+      <c r="M31" s="27">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="N31" s="4">
         <f t="shared" si="1"/>
-        <v>0.31944444444444448</v>
+        <v>0.4861111111111111</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="6">
+      <c r="B32" s="4">
         <f t="shared" ref="B32:M32" si="2">SUM(B2:B31)</f>
-        <v>3.6006944444444446</v>
-      </c>
-      <c r="C32" s="6">
+        <v>3.8611111111111112</v>
+      </c>
+      <c r="C32" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333337</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333337</v>
       </c>
-      <c r="I32" s="6">
+      <c r="I32" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333337</v>
       </c>
-      <c r="J32" s="6">
+      <c r="J32" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333337</v>
       </c>
-      <c r="K32" s="6">
+      <c r="K32" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="L32" s="6">
+      <c r="L32" s="4">
         <f t="shared" si="2"/>
         <v>0.33333333333333337</v>
       </c>
-      <c r="M32" s="6">
+      <c r="M32" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="33" spans="13:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M33" s="6">
+      <c r="M33" s="4">
         <f>SUM(C32:M32)</f>
-        <v>3.3333333333333339</v>
-      </c>
-      <c r="N33" s="6">
+        <v>3.6666666666666674</v>
+      </c>
+      <c r="N33" s="4">
         <f>SUM(N2:N31)</f>
-        <v>3.1875000000000004</v>
+        <v>3.666666666666667</v>
       </c>
     </row>
     <row r="34" spans="13:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>